<commit_message>
Updated SPP subgoal with ESA scores and fish biomass scores
</commit_message>
<xml_diff>
--- a/prep/SPP/spp_ESA_status.xlsx
+++ b/prep/SPP/spp_ESA_status.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7320" yWindow="-120" windowWidth="19155" windowHeight="6720"/>
+    <workbookView xWindow="540" yWindow="300" windowWidth="19155" windowHeight="6720"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -719,11 +719,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1028,14 +1029,14 @@
   <dimension ref="A1:D105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.85546875" customWidth="1"/>
+    <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="31.140625" customWidth="1"/>
-    <col min="3" max="4" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1048,7 +1049,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1063,7 +1064,7 @@
         <v>6</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1077,7 +1078,7 @@
         <v>9</v>
       </c>
       <c r="D3">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1091,7 +1092,7 @@
         <v>6</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1105,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1119,7 +1120,7 @@
         <v>6</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1133,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1147,7 +1148,7 @@
         <v>9</v>
       </c>
       <c r="D8">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1161,7 +1162,7 @@
         <v>9</v>
       </c>
       <c r="D9">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1175,7 +1176,7 @@
         <v>6</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1189,7 +1190,7 @@
         <v>26</v>
       </c>
       <c r="D11">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1203,7 +1204,7 @@
         <v>9</v>
       </c>
       <c r="D12">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1217,7 +1218,7 @@
         <v>9</v>
       </c>
       <c r="D13">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1231,7 +1232,7 @@
         <v>9</v>
       </c>
       <c r="D14">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1245,7 +1246,7 @@
         <v>6</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1259,7 +1260,7 @@
         <v>9</v>
       </c>
       <c r="D16">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1273,7 +1274,7 @@
         <v>9</v>
       </c>
       <c r="D17">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1287,7 +1288,7 @@
         <v>6</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1301,7 +1302,7 @@
         <v>6</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1315,7 +1316,7 @@
         <v>6</v>
       </c>
       <c r="D20">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1329,7 +1330,7 @@
         <v>6</v>
       </c>
       <c r="D21">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1343,7 +1344,7 @@
         <v>26</v>
       </c>
       <c r="D22">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1357,7 +1358,7 @@
         <v>6</v>
       </c>
       <c r="D23">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1371,7 +1372,7 @@
         <v>6</v>
       </c>
       <c r="D24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1385,7 +1386,7 @@
         <v>6</v>
       </c>
       <c r="D25">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1399,7 +1400,7 @@
         <v>6</v>
       </c>
       <c r="D26">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1413,7 +1414,7 @@
         <v>6</v>
       </c>
       <c r="D27">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1427,7 +1428,7 @@
         <v>9</v>
       </c>
       <c r="D28">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1441,7 +1442,7 @@
         <v>6</v>
       </c>
       <c r="D29">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1455,7 +1456,7 @@
         <v>9</v>
       </c>
       <c r="D30">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1469,7 +1470,7 @@
         <v>6</v>
       </c>
       <c r="D31">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -1483,7 +1484,7 @@
         <v>6</v>
       </c>
       <c r="D32">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1494,7 +1495,7 @@
         <v>86</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1505,7 +1506,7 @@
         <v>87</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1519,7 +1520,7 @@
         <v>9</v>
       </c>
       <c r="D35">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1530,7 +1531,7 @@
         <v>89</v>
       </c>
       <c r="D36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -1541,7 +1542,7 @@
         <v>90</v>
       </c>
       <c r="D37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -1552,7 +1553,7 @@
         <v>91</v>
       </c>
       <c r="D38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1563,7 +1564,7 @@
         <v>92</v>
       </c>
       <c r="D39">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1574,7 +1575,7 @@
         <v>93</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1585,7 +1586,7 @@
         <v>94</v>
       </c>
       <c r="D41">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1596,7 +1597,7 @@
         <v>95</v>
       </c>
       <c r="D42">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1607,7 +1608,7 @@
         <v>96</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1618,7 +1619,7 @@
         <v>97</v>
       </c>
       <c r="D44">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1629,7 +1630,7 @@
         <v>98</v>
       </c>
       <c r="D45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1640,7 +1641,7 @@
         <v>99</v>
       </c>
       <c r="D46">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1651,7 +1652,7 @@
         <v>100</v>
       </c>
       <c r="D47">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1662,7 +1663,7 @@
         <v>101</v>
       </c>
       <c r="D48">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1673,7 +1674,7 @@
         <v>102</v>
       </c>
       <c r="D49">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,7 +1688,7 @@
         <v>212</v>
       </c>
       <c r="D50">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1698,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="D51">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1712,7 +1713,7 @@
         <v>212</v>
       </c>
       <c r="D52">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1723,7 +1724,7 @@
         <v>159</v>
       </c>
       <c r="D53">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1737,7 +1738,7 @@
         <v>212</v>
       </c>
       <c r="D54">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1748,7 +1749,7 @@
         <v>161</v>
       </c>
       <c r="D55">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1762,7 +1763,7 @@
         <v>212</v>
       </c>
       <c r="D56">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1776,7 +1777,7 @@
         <v>213</v>
       </c>
       <c r="D57">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1790,7 +1791,7 @@
         <v>212</v>
       </c>
       <c r="D58">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1804,7 +1805,7 @@
         <v>213</v>
       </c>
       <c r="D59">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1818,7 +1819,7 @@
         <v>212</v>
       </c>
       <c r="D60">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1832,7 +1833,7 @@
         <v>213</v>
       </c>
       <c r="D61">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1846,7 +1847,7 @@
         <v>213</v>
       </c>
       <c r="D62">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -1860,7 +1861,7 @@
         <v>212</v>
       </c>
       <c r="D63">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -1874,7 +1875,7 @@
         <v>213</v>
       </c>
       <c r="D64">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1889,7 @@
         <v>213</v>
       </c>
       <c r="D65">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -1899,7 +1900,7 @@
         <v>172</v>
       </c>
       <c r="D66">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -1913,7 +1914,7 @@
         <v>212</v>
       </c>
       <c r="D67">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,7 +1928,7 @@
         <v>213</v>
       </c>
       <c r="D68">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -1941,7 +1942,7 @@
         <v>213</v>
       </c>
       <c r="D69">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,7 +1953,7 @@
         <v>176</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -1963,7 +1964,7 @@
         <v>177</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -1974,7 +1975,7 @@
         <v>178</v>
       </c>
       <c r="D72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -1985,7 +1986,7 @@
         <v>179</v>
       </c>
       <c r="D73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -1996,7 +1997,7 @@
         <v>180</v>
       </c>
       <c r="D74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -2007,7 +2008,7 @@
         <v>181</v>
       </c>
       <c r="D75">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -2018,7 +2019,7 @@
         <v>182</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -2029,7 +2030,7 @@
         <v>183</v>
       </c>
       <c r="D77">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -2040,7 +2041,7 @@
         <v>184</v>
       </c>
       <c r="D78">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -2051,7 +2052,7 @@
         <v>185</v>
       </c>
       <c r="D79">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -2062,7 +2063,7 @@
         <v>186</v>
       </c>
       <c r="D80">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -2073,7 +2074,7 @@
         <v>187</v>
       </c>
       <c r="D81">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -2084,7 +2085,7 @@
         <v>188</v>
       </c>
       <c r="D82">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -2095,7 +2096,7 @@
         <v>189</v>
       </c>
       <c r="D83">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -2106,7 +2107,7 @@
         <v>190</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -2117,7 +2118,7 @@
         <v>191</v>
       </c>
       <c r="D85">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -2128,7 +2129,7 @@
         <v>192</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -2139,7 +2140,7 @@
         <v>193</v>
       </c>
       <c r="D87">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -2150,7 +2151,7 @@
         <v>194</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -2161,7 +2162,7 @@
         <v>195</v>
       </c>
       <c r="D89">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -2172,7 +2173,7 @@
         <v>196</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -2183,7 +2184,7 @@
         <v>197</v>
       </c>
       <c r="D91">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -2194,7 +2195,7 @@
         <v>198</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -2205,7 +2206,7 @@
         <v>199</v>
       </c>
       <c r="D93">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -2216,7 +2217,7 @@
         <v>200</v>
       </c>
       <c r="D94">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -2227,7 +2228,7 @@
         <v>201</v>
       </c>
       <c r="D95">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -2238,7 +2239,7 @@
         <v>202</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -2249,7 +2250,7 @@
         <v>203</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -2260,7 +2261,7 @@
         <v>204</v>
       </c>
       <c r="D98">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -2271,7 +2272,7 @@
         <v>205</v>
       </c>
       <c r="D99">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -2285,7 +2286,7 @@
         <v>213</v>
       </c>
       <c r="D100">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -2296,7 +2297,7 @@
         <v>207</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -2307,7 +2308,7 @@
         <v>208</v>
       </c>
       <c r="D102">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -2318,7 +2319,7 @@
         <v>209</v>
       </c>
       <c r="D103">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -2329,7 +2330,7 @@
         <v>210</v>
       </c>
       <c r="D104">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -2340,7 +2341,7 @@
         <v>211</v>
       </c>
       <c r="D105">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>